<commit_message>
Add in workflow to convert to transcript
</commit_message>
<xml_diff>
--- a/tools/gdc_video_data.xlsx
+++ b/tools/gdc_video_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\GDC-transcript\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DBEF2A-21FE-4A31-9C7D-EF94DE4E3AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAD59E4-FD59-48CA-BF08-FCBA3F932748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{45A17641-AF43-48ED-A0AC-BE5F2E65EF92}"/>
+    <workbookView xWindow="45972" yWindow="1572" windowWidth="30936" windowHeight="16776" xr2:uid="{45A17641-AF43-48ED-A0AC-BE5F2E65EF92}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3477" uniqueCount="3475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3480" uniqueCount="3477">
   <si>
     <t>title</t>
   </si>
@@ -10484,6 +10484,14 @@
   </si>
   <si>
     <t>IGF 2023: Marina Díez Host Announcement</t>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欄1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -10540,7 +10548,10 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -10571,23 +10582,25 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="外部資料_1" connectionId="4" xr16:uid="{17105E8F-8C1C-40CE-B1DE-0BA481E77C3F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="4">
-    <queryTableFields count="3">
+  <queryTableRefresh nextId="5" unboundColumnsRight="1">
+    <queryTableFields count="4">
       <queryTableField id="1" name="title" tableColumnId="1"/>
       <queryTableField id="2" name="video_id" tableColumnId="2"/>
       <queryTableField id="3" name="view_count" tableColumnId="3"/>
+      <queryTableField id="4" dataBound="0" tableColumnId="4"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D499193A-6E77-44AB-A9B1-AF972C15029D}" name="video_data_sorted__4" displayName="video_data_sorted__4" ref="A1:C1738" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:C1738" xr:uid="{D499193A-6E77-44AB-A9B1-AF972C15029D}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0EBFDFD6-2F00-4FE3-9B05-96879654692F}" uniqueName="1" name="title" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{D523D53E-0D48-4657-AACB-D17090CE6301}" uniqueName="2" name="video_id" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{03EE52D8-B606-450F-B691-7A3A5D4D3AC6}" uniqueName="3" name="view_count" queryTableFieldId="3" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D499193A-6E77-44AB-A9B1-AF972C15029D}" name="video_data_sorted__4" displayName="video_data_sorted__4" ref="A1:D1738" tableType="queryTable" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D1738" xr:uid="{D499193A-6E77-44AB-A9B1-AF972C15029D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0EBFDFD6-2F00-4FE3-9B05-96879654692F}" uniqueName="1" name="title" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D523D53E-0D48-4657-AACB-D17090CE6301}" uniqueName="2" name="video_id" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{03EE52D8-B606-450F-B691-7A3A5D4D3AC6}" uniqueName="3" name="view_count" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{E38AB26E-C418-43A8-9482-5A0CA9F2D8F9}" uniqueName="4" name="欄1" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10890,10 +10903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1CF3E4-52BD-48CE-81E9-C5104775D7E1}">
-  <dimension ref="A1:C1738"/>
+  <dimension ref="A1:D1738"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
+      <selection activeCell="B251" sqref="B251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.75" x14ac:dyDescent="0.45"/>
@@ -10904,7 +10917,7 @@
     <col min="4" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10914,8 +10927,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" s="1" t="s">
+        <v>3476</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -10926,7 +10942,7 @@
         <v>1487665</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -10937,7 +10953,7 @@
         <v>1461399</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -10948,7 +10964,7 @@
         <v>1034205</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -10959,7 +10975,7 @@
         <v>1032480</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -10970,7 +10986,7 @@
         <v>968859</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -10981,7 +10997,7 @@
         <v>868086</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -10992,7 +11008,7 @@
         <v>840359</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -11003,7 +11019,7 @@
         <v>702961</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -11014,7 +11030,7 @@
         <v>685210</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -11025,7 +11041,7 @@
         <v>668791</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -11036,7 +11052,7 @@
         <v>629179</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -11047,7 +11063,7 @@
         <v>608761</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -11058,7 +11074,7 @@
         <v>588999</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -11069,7 +11085,7 @@
         <v>548935</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -13016,7 +13032,7 @@
         <v>61410</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A193" s="1" t="s">
         <v>385</v>
       </c>
@@ -13027,7 +13043,7 @@
         <v>60676</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A194" s="1" t="s">
         <v>387</v>
       </c>
@@ -13038,7 +13054,7 @@
         <v>58375</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A195" s="1" t="s">
         <v>389</v>
       </c>
@@ -13049,7 +13065,7 @@
         <v>57544</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A196" s="1" t="s">
         <v>391</v>
       </c>
@@ -13060,7 +13076,7 @@
         <v>57459</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A197" s="1" t="s">
         <v>393</v>
       </c>
@@ -13071,7 +13087,7 @@
         <v>56016</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A198" s="1" t="s">
         <v>395</v>
       </c>
@@ -13082,7 +13098,7 @@
         <v>56010</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A199" s="1" t="s">
         <v>397</v>
       </c>
@@ -13093,7 +13109,7 @@
         <v>55961</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A200" s="1" t="s">
         <v>399</v>
       </c>
@@ -13103,8 +13119,11 @@
       <c r="C200" s="1">
         <v>55642</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D200" s="1" t="s">
+        <v>3475</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A201" s="1" t="s">
         <v>401</v>
       </c>
@@ -13115,7 +13134,7 @@
         <v>54939</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A202" s="1" t="s">
         <v>403</v>
       </c>
@@ -13126,7 +13145,7 @@
         <v>54466</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A203" s="1" t="s">
         <v>405</v>
       </c>
@@ -13137,7 +13156,7 @@
         <v>54176</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A204" s="1" t="s">
         <v>407</v>
       </c>
@@ -13148,7 +13167,7 @@
         <v>54073</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A205" s="1" t="s">
         <v>409</v>
       </c>
@@ -13159,7 +13178,7 @@
         <v>53869</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A206" s="1" t="s">
         <v>411</v>
       </c>
@@ -13170,7 +13189,7 @@
         <v>53809</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A207" s="1" t="s">
         <v>413</v>
       </c>
@@ -13181,7 +13200,7 @@
         <v>53742</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A208" s="1" t="s">
         <v>415</v>
       </c>
@@ -13544,7 +13563,7 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A241" s="1" t="s">
         <v>480</v>
       </c>
@@ -13555,7 +13574,7 @@
         <v>45426</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A242" s="1" t="s">
         <v>482</v>
       </c>
@@ -13566,7 +13585,7 @@
         <v>45250</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A243" s="1" t="s">
         <v>484</v>
       </c>
@@ -13577,7 +13596,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A244" s="1" t="s">
         <v>486</v>
       </c>
@@ -13588,7 +13607,7 @@
         <v>45137</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A245" s="1" t="s">
         <v>488</v>
       </c>
@@ -13599,7 +13618,7 @@
         <v>44511</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A246" s="1" t="s">
         <v>490</v>
       </c>
@@ -13610,7 +13629,7 @@
         <v>44464</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A247" s="1" t="s">
         <v>492</v>
       </c>
@@ -13621,7 +13640,7 @@
         <v>44338</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A248" s="1" t="s">
         <v>494</v>
       </c>
@@ -13632,7 +13651,7 @@
         <v>44009</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A249" s="1" t="s">
         <v>496</v>
       </c>
@@ -13643,7 +13662,7 @@
         <v>43925</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A250" s="1" t="s">
         <v>498</v>
       </c>
@@ -13653,8 +13672,11 @@
       <c r="C250" s="1">
         <v>43787</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D250" s="1" t="s">
+        <v>3475</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A251" s="1" t="s">
         <v>500</v>
       </c>
@@ -13665,7 +13687,7 @@
         <v>43787</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A252" s="1" t="s">
         <v>502</v>
       </c>
@@ -13676,7 +13698,7 @@
         <v>43508</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A253" s="1" t="s">
         <v>504</v>
       </c>
@@ -13687,7 +13709,7 @@
         <v>42810</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A254" s="1" t="s">
         <v>506</v>
       </c>
@@ -13698,7 +13720,7 @@
         <v>42520</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A255" s="1" t="s">
         <v>508</v>
       </c>
@@ -13709,7 +13731,7 @@
         <v>42170</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A256" s="1" t="s">
         <v>510</v>
       </c>

</xml_diff>